<commit_message>
accidents endpoints added, but those endpoints are not 100% done
</commit_message>
<xml_diff>
--- a/docs/endpoints.xlsx
+++ b/docs/endpoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\diagrams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0005D40A-0756-4C8C-B2FC-D6D234ADCC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871522C0-EF29-4FB0-B3C8-CE2BB0089D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7545" yWindow="7185" windowWidth="14445" windowHeight="10275" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
+    <workbookView xWindow="1215" yWindow="4410" windowWidth="14340" windowHeight="10275" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="81">
   <si>
     <t>Klasa</t>
   </si>
@@ -182,9 +182,6 @@
     <t>update_milage</t>
   </si>
   <si>
-    <t>/api/accidents/{date}/{type}</t>
-  </si>
-  <si>
     <t>/api/shifts/{shift_id}</t>
   </si>
   <si>
@@ -218,9 +215,6 @@
     <t>/api/cars/{car_id}</t>
   </si>
   <si>
-    <t>/api/accidents{accident_id}</t>
-  </si>
-  <si>
     <t>/api/availability/{data}/{type}</t>
   </si>
   <si>
@@ -276,6 +270,15 @@
   </si>
   <si>
     <t>submit</t>
+  </si>
+  <si>
+    <t>/api/accidents/{accident_id}</t>
+  </si>
+  <si>
+    <t>/api/accidents/find</t>
+  </si>
+  <si>
+    <t>find</t>
   </si>
 </sst>
 </file>
@@ -660,7 +663,7 @@
   <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +711,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
@@ -728,10 +731,10 @@
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -774,7 +777,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>33</v>
@@ -797,10 +800,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
@@ -843,7 +846,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>34</v>
@@ -889,7 +892,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>36</v>
@@ -935,7 +938,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>37</v>
@@ -981,7 +984,7 @@
         <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>43</v>
@@ -1001,10 +1004,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
@@ -1019,13 +1022,13 @@
         <v>2</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
@@ -1126,7 +1129,7 @@
         <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>11</v>
@@ -1149,7 +1152,7 @@
         <v>17</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
@@ -1172,7 +1175,7 @@
         <v>17</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
@@ -1192,10 +1195,10 @@
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
@@ -1218,7 +1221,7 @@
         <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -1238,10 +1241,10 @@
         <v>32</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
@@ -1307,7 +1310,7 @@
         <v>32</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>33</v>
@@ -1353,7 +1356,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>34</v>
@@ -1399,7 +1402,7 @@
         <v>35</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>36</v>
@@ -1422,7 +1425,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>47</v>
@@ -1445,7 +1448,7 @@
         <v>8</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>22</v>
@@ -1468,7 +1471,7 @@
         <v>12</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>40</v>
@@ -1488,13 +1491,13 @@
         <v>20</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>14</v>
@@ -1530,17 +1533,17 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="B47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>53</v>
+      <c r="D47" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>11</v>
@@ -1548,8 +1551,8 @@
       <c r="F47" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G47" s="1">
-        <v>0</v>
+      <c r="G47" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1563,7 +1566,7 @@
         <v>23</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>11</v>
@@ -1576,17 +1579,17 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>62</v>
+      <c r="B49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>14</v>
@@ -1594,7 +1597,7 @@
       <c r="F49" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G49" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1609,7 +1612,7 @@
         <v>12</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>24</v>
@@ -1632,7 +1635,7 @@
         <v>32</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>27</v>
@@ -1655,7 +1658,7 @@
         <v>12</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>28</v>
@@ -1678,10 +1681,10 @@
         <v>8</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>14</v>
@@ -1701,10 +1704,10 @@
         <v>32</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>14</v>
@@ -1724,10 +1727,10 @@
         <v>12</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>14</v>
@@ -1747,7 +1750,7 @@
         <v>12</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>24</v>
@@ -1770,7 +1773,7 @@
         <v>12</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
All email endpoints done
</commit_message>
<xml_diff>
--- a/docs/endpoints.xlsx
+++ b/docs/endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492EC34A-100A-41E4-987E-FA29AF78B296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D27D8A5-8CE9-4234-AEB1-8DFDAB5A992B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="156">
   <si>
     <t>Klasa</t>
   </si>
@@ -188,9 +188,6 @@
     <t>User</t>
   </si>
   <si>
-    <t>List&lt;User&gt;</t>
-  </si>
-  <si>
     <t>Void</t>
   </si>
   <si>
@@ -371,9 +368,6 @@
     <t>/api/shifts (date, type w body)</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Podaj poprawny adres email.</t>
   </si>
   <si>
@@ -404,9 +398,6 @@
     <t>UserRequest</t>
   </si>
   <si>
-    <t>UserLoginData</t>
-  </si>
-  <si>
     <t>/api/users</t>
   </si>
   <si>
@@ -498,6 +489,21 @@
   </si>
   <si>
     <t>Podaj poprawne dane. | Aktywuj konto. | Twoje konto jest zablokowane, skontakuj się z administratorem.</t>
+  </si>
+  <si>
+    <t>EmailRequest</t>
+  </si>
+  <si>
+    <t>UserResponse</t>
+  </si>
+  <si>
+    <t>EmailResponse</t>
+  </si>
+  <si>
+    <t>List&lt;UserResponse&gt;</t>
+  </si>
+  <si>
+    <t>UserLoginDataRequest</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1022,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,7 +1034,7 @@
     <col min="5" max="5" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="255.5703125" style="2" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="2"/>
@@ -1054,16 +1060,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>48</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -1074,10 +1080,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>8</v>
@@ -1089,13 +1095,13 @@
         <v>11</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I2" s="27" t="s">
         <v>49</v>
       </c>
       <c r="J2" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -1106,10 +1112,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E3" s="31" t="s">
         <v>8</v>
@@ -1121,13 +1127,13 @@
         <v>3</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>122</v>
+        <v>155</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>49</v>
+        <v>152</v>
       </c>
       <c r="J3" s="31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -1138,10 +1144,10 @@
         <v>26</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E4" s="31" t="s">
         <v>8</v>
@@ -1153,13 +1159,13 @@
         <v>2</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -1170,10 +1176,10 @@
         <v>26</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>11</v>
@@ -1185,13 +1191,13 @@
         <v>2</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I5" s="23" t="s">
         <v>49</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -1202,10 +1208,10 @@
         <v>26</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>11</v>
@@ -1217,13 +1223,13 @@
         <v>2</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I6" s="23" t="s">
         <v>49</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -1234,10 +1240,10 @@
         <v>26</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>11</v>
@@ -1249,13 +1255,13 @@
         <v>2</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I7" s="23" t="s">
         <v>49</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -1266,10 +1272,10 @@
         <v>26</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>11</v>
@@ -1281,13 +1287,13 @@
         <v>2</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>49</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -1298,10 +1304,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>11</v>
@@ -1313,10 +1319,10 @@
         <v>0</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="J9" s="22"/>
     </row>
@@ -1328,10 +1334,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>11</v>
@@ -1343,10 +1349,10 @@
         <v>0</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="J10" s="25"/>
     </row>
@@ -1358,10 +1364,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>11</v>
@@ -1373,10 +1379,10 @@
         <v>0</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="J11" s="7"/>
     </row>
@@ -1388,10 +1394,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>11</v>
@@ -1403,10 +1409,10 @@
         <v>0</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="J12" s="22"/>
     </row>
@@ -1418,10 +1424,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>11</v>
@@ -1433,10 +1439,10 @@
         <v>0</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="J13" s="22"/>
     </row>
@@ -1448,10 +1454,10 @@
         <v>29</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E14" s="29" t="s">
         <v>11</v>
@@ -1463,13 +1469,13 @@
         <v>1</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I14" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J14" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -1480,10 +1486,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>8</v>
@@ -1495,13 +1501,13 @@
         <v>1</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J15" s="31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1515,7 +1521,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>25</v>
@@ -1530,13 +1536,13 @@
         <v>3</v>
       </c>
       <c r="H17" s="23" t="s">
-        <v>77</v>
+        <v>151</v>
       </c>
       <c r="I17" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="J17" s="22" t="s">
         <v>111</v>
-      </c>
-      <c r="J17" s="22" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -1547,7 +1553,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>30</v>
@@ -1562,13 +1568,13 @@
         <v>1</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>77</v>
+        <v>151</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J18" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1582,7 +1588,7 @@
         <v>9</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>21</v>
@@ -1598,10 +1604,10 @@
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1612,7 +1618,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>13</v>
@@ -1628,10 +1634,10 @@
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1642,7 +1648,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>14</v>
@@ -1658,10 +1664,10 @@
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1672,10 +1678,10 @@
         <v>9</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>11</v>
@@ -1688,10 +1694,10 @@
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1702,7 +1708,7 @@
         <v>9</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>40</v>
@@ -1718,10 +1724,10 @@
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="J24" s="18" t="s">
         <v>107</v>
-      </c>
-      <c r="J24" s="18" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1732,10 +1738,10 @@
         <v>26</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>11</v>
@@ -1749,7 +1755,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="20"/>
       <c r="J25" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1779,10 +1785,10 @@
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1793,7 +1799,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>32</v>
@@ -1809,7 +1815,7 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J28" s="7"/>
     </row>
@@ -1821,7 +1827,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>27</v>
@@ -1837,10 +1843,10 @@
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1851,7 +1857,7 @@
         <v>9</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>31</v>
@@ -1867,7 +1873,7 @@
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J30" s="7"/>
     </row>
@@ -1879,7 +1885,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>28</v>
@@ -1895,10 +1901,10 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1909,7 +1915,7 @@
         <v>9</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>33</v>
@@ -1925,7 +1931,7 @@
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J32" s="7"/>
     </row>
@@ -1937,7 +1943,7 @@
         <v>29</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>30</v>
@@ -1953,10 +1959,10 @@
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1967,7 +1973,7 @@
         <v>26</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>36</v>
@@ -1983,10 +1989,10 @@
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1997,10 +2003,10 @@
         <v>9</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>11</v>
@@ -2012,10 +2018,10 @@
         <v>1</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2045,10 +2051,10 @@
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2059,7 +2065,7 @@
         <v>9</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>33</v>
@@ -2075,10 +2081,10 @@
       </c>
       <c r="H38" s="10"/>
       <c r="I38" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J38" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2089,7 +2095,7 @@
         <v>9</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>47</v>
@@ -2105,10 +2111,10 @@
       </c>
       <c r="H39" s="10"/>
       <c r="I39" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2138,10 +2144,10 @@
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J41" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2152,7 +2158,7 @@
         <v>9</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>38</v>
@@ -2168,10 +2174,10 @@
       </c>
       <c r="H42" s="9"/>
       <c r="I42" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J42" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2198,10 +2204,10 @@
       </c>
       <c r="H43" s="15"/>
       <c r="I43" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J43" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2212,10 +2218,10 @@
         <v>9</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>11</v>
@@ -2228,10 +2234,10 @@
       </c>
       <c r="H44" s="17"/>
       <c r="I44" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J44" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2246,7 +2252,7 @@
         <v>9</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>19</v>
@@ -2262,10 +2268,10 @@
       </c>
       <c r="H46" s="9"/>
       <c r="I46" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2276,7 +2282,7 @@
         <v>26</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>22</v>
@@ -2292,10 +2298,10 @@
       </c>
       <c r="H47" s="9"/>
       <c r="I47" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2306,7 +2312,7 @@
         <v>9</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>23</v>
@@ -2322,10 +2328,10 @@
       </c>
       <c r="H48" s="9"/>
       <c r="I48" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2352,10 +2358,10 @@
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2382,10 +2388,10 @@
       </c>
       <c r="H50" s="10"/>
       <c r="I50" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2399,7 +2405,7 @@
         <v>44</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>11</v>
@@ -2412,7 +2418,7 @@
       </c>
       <c r="H51" s="10"/>
       <c r="I51" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J51" s="7"/>
     </row>
@@ -2430,7 +2436,7 @@
         <v>39</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>8</v>
@@ -2443,10 +2449,10 @@
       </c>
       <c r="H53" s="9"/>
       <c r="I53" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2457,10 +2463,10 @@
         <v>9</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>8</v>
@@ -2473,10 +2479,10 @@
       </c>
       <c r="H54" s="9"/>
       <c r="I54" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2487,10 +2493,10 @@
         <v>9</v>
       </c>
       <c r="C55" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>11</v>
@@ -2503,10 +2509,10 @@
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All shift endpoints done
</commit_message>
<xml_diff>
--- a/docs/endpoints.xlsx
+++ b/docs/endpoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019573B3-269E-4598-813B-497791633BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521915F8-FA44-4F61-9BDF-CAE2F1B5E7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="10545" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
+    <workbookView xWindow="0" yWindow="330" windowWidth="38700" windowHeight="15345" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="180">
   <si>
     <t>Klasa</t>
   </si>
@@ -77,12 +77,6 @@
     <t>availability</t>
   </si>
   <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
     <t>accident</t>
   </si>
   <si>
@@ -110,9 +104,6 @@
     <t>/api/accidents/{shift_id}</t>
   </si>
   <si>
-    <t>get_complex_info</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -131,18 +122,6 @@
     <t>Błedy</t>
   </si>
   <si>
-    <t>Shift</t>
-  </si>
-  <si>
-    <t>/api/shifts/{user_id}</t>
-  </si>
-  <si>
-    <t>/api/shifts/{id}</t>
-  </si>
-  <si>
-    <t>Accident</t>
-  </si>
-  <si>
     <t>Brak zmiany o {shift_id} | Załącz minimum 4 zdjęcia pokazujące uszkodzenia | Załącz minimum 1 zdjęcie dokumentów | Podaj przebieg auta | Podaj poprawny przebieg auta</t>
   </si>
   <si>
@@ -164,39 +143,15 @@
     <t>Integer</t>
   </si>
   <si>
-    <t>List&lt;AccidentExtended&gt;</t>
-  </si>
-  <si>
     <t>/api/accidents (date, type w body)</t>
   </si>
   <si>
-    <t>AccidentExtended</t>
-  </si>
-  <si>
-    <t>update_fuel_consumption</t>
-  </si>
-  <si>
     <t>Brak wypadku o id {id}</t>
   </si>
   <si>
     <t>List&lt;SettlementsExtended&gt;</t>
   </si>
   <si>
-    <t>/api/cars/{id} (lpg, petrol w body)</t>
-  </si>
-  <si>
-    <t>find_all_shifts_in_day_of_current_type</t>
-  </si>
-  <si>
-    <t>List&lt;ExtendedShift&gt;</t>
-  </si>
-  <si>
-    <t>ExtendedShift</t>
-  </si>
-  <si>
-    <t>/api/shifts (date, type w body)</t>
-  </si>
-  <si>
     <t>Podaj poprawny adres email.</t>
   </si>
   <si>
@@ -548,23 +503,86 @@
     <t>Brak zmiany o id {id}.</t>
   </si>
   <si>
-    <t>Załącz minimum 8 zdjęć auta z zewnątrz. | Załącz zdjęcie przebiegu. | Podaj przebieg auta. | Podaj poprawny przebieg auta. |  Brak użytkownika o {id}.</t>
-  </si>
-  <si>
-    <t>Załącz minimum 8 zdjęć auta z zewnątrz. | Załącz zdjęcie przebiegu. | Podaj przebieg auta. | Podaj poprawny przebieg auta. | Podaj ile litrów gazu spaliło auta.| Podaj poprawnie ile litrów gazu spaliło auto | Podaj ile litrów benzyny spaliło auto | Podaj poprawnie ile litrów benzyny spaliło auto | Załącz zdjęcie faktury. |  Brak zmiany o {id}.</t>
-  </si>
-  <si>
-    <t>Brak zmiany od id {id}.</t>
-  </si>
-  <si>
-    <t>Brak zmiany o id {id}. | Podaj ile litrów gazu spaliło auta. | Podaj poprawnie ile litrów gazu spaliło auto. | Podaj ile litrów benzyny spaliło auto. | Podaj poprawnie ile litrów benzyny spaliło auto.</t>
+    <t>/api/shifts/start</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>StartShiftRequest</t>
+  </si>
+  <si>
+    <t>EndShiftRequest</t>
+  </si>
+  <si>
+    <t>ShiftResponse</t>
+  </si>
+  <si>
+    <t>FuelRequest</t>
+  </si>
+  <si>
+    <t>Update fuel consumption</t>
+  </si>
+  <si>
+    <t>List&lt;ShiftResponse&gt;</t>
+  </si>
+  <si>
+    <t>/api/shifts/find</t>
+  </si>
+  <si>
+    <t>ExtendedShiftResponse</t>
+  </si>
+  <si>
+    <t>/api/shifts/info/{id}</t>
+  </si>
+  <si>
+    <t>Find all by day and type</t>
+  </si>
+  <si>
+    <t>/api/shifts/end</t>
+  </si>
+  <si>
+    <t>/api/shifts/update_fuel</t>
+  </si>
+  <si>
+    <t>List&lt;ExtendedAccidentResponse&gt;</t>
+  </si>
+  <si>
+    <t>ExtendedAccidentResponse</t>
+  </si>
+  <si>
+    <t>AccidentResponse</t>
+  </si>
+  <si>
+    <t>Brak zmiany od id {id}. | Zmiana o id {id} nie została jeszcze zakończona.</t>
+  </si>
+  <si>
+    <t>Brak zmiany o id {id}. | Podaj ile litrów gazu spaliło auta. | Podaj poprawnie ile litrów gazu spaliło auto. | Podaj ile litrów benzyny spaliło auto. | Podaj poprawnie ile litrów benzyny spaliło auto. | Zmiana o id {id} nie została jeszcze zakończona.</t>
+  </si>
+  <si>
+    <t>/api/shifts/generate</t>
+  </si>
+  <si>
+    <t>Generate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zmiany na następny tydzień zostały już wygenerowane. | Zmiany na następny tydzień będą mogły być wygenerowane dopiero w piątek. </t>
+  </si>
+  <si>
+    <t>Załącz minimum 8 zdjęć auta z zewnątrz. | Załącz zdjęcie przebiegu. | Podaj przebieg auta. | Podaj poprawny przebieg auta. | Użytkownik o id {id} nie został przydzielony do rozpoczęcia zmiany {data} {typ}. | Brak użytkownika o id {id}. | Zmiana od id {id} została już rozpoczęta. | Zmiana od id {id} została już zakończona.</t>
+  </si>
+  <si>
+    <t>Załącz minimum 8 zdjęć auta z zewnątrz. | Załącz zdjęcie przebiegu. | Podaj przebieg auta. | Podaj poprawny przebieg auta. | Podaj ile litrów gazu spaliło auta.| Podaj poprawnie ile litrów gazu spaliło auto | Podaj ile litrów benzyny spaliło auto | Podaj poprawnie ile litrów benzyny spaliło auto | Załącz zdjęcie faktury. | Brak zmiany o {id}. | Zmiana o id {id} nie została jeszcze rozpoczęta. | Zmiana od id {id} została już zakończona.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +642,15 @@
       <b/>
       <u/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -736,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -771,6 +798,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1085,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1555BF42-8AEC-4F54-8DDE-B70EA6966B6F}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,9 +1135,10 @@
     <col min="6" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="255.42578125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="9.140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1126,16 +1161,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>30</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -1146,10 +1181,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>8</v>
@@ -1161,13 +1196,13 @@
         <v>11</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1178,10 +1213,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>8</v>
@@ -1193,13 +1228,13 @@
         <v>3</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1207,13 +1242,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>8</v>
@@ -1225,13 +1260,13 @@
         <v>2</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -1239,13 +1274,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>11</v>
@@ -1257,13 +1292,13 @@
         <v>2</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -1271,13 +1306,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>11</v>
@@ -1289,13 +1324,13 @@
         <v>2</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -1303,13 +1338,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>11</v>
@@ -1321,13 +1356,13 @@
         <v>2</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -1335,13 +1370,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>11</v>
@@ -1353,13 +1388,13 @@
         <v>2</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -1370,10 +1405,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>11</v>
@@ -1385,10 +1420,10 @@
         <v>0</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="J9" s="17"/>
     </row>
@@ -1400,10 +1435,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>82</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>11</v>
@@ -1415,10 +1450,10 @@
         <v>0</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="J10" s="24"/>
     </row>
@@ -1430,10 +1465,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>83</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>11</v>
@@ -1445,10 +1480,10 @@
         <v>0</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="J11" s="26"/>
     </row>
@@ -1460,10 +1495,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>11</v>
@@ -1475,10 +1510,10 @@
         <v>0</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="J12" s="17"/>
     </row>
@@ -1490,10 +1525,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>11</v>
@@ -1505,10 +1540,10 @@
         <v>0</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="J13" s="17"/>
     </row>
@@ -1517,13 +1552,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="E14" s="27" t="s">
         <v>11</v>
@@ -1535,13 +1570,13 @@
         <v>1</v>
       </c>
       <c r="H14" s="28" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1552,10 +1587,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>8</v>
@@ -1567,13 +1602,13 @@
         <v>1</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1581,16 +1616,16 @@
     </row>
     <row r="17" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>11</v>
@@ -1602,27 +1637,27 @@
         <v>3</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>11</v>
@@ -1634,275 +1669,287 @@
         <v>1</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="34">
+        <v>2</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="34">
+        <v>8</v>
+      </c>
+      <c r="H21" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="I21" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C22" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="34">
+        <v>1</v>
+      </c>
+      <c r="H22" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="I22" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="34">
+        <v>12</v>
+      </c>
+      <c r="H23" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="I23" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="J23" s="34" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="D24" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="3">
-        <v>1</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J20" s="3" t="s">
+      <c r="E24" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="37">
+        <v>0</v>
+      </c>
+      <c r="H24" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I24" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="J24" s="39"/>
+    </row>
+    <row r="25" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="37">
+        <v>2</v>
+      </c>
+      <c r="H25" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="I25" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="J25" s="37" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="37" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="D26" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="37">
+        <v>6</v>
+      </c>
+      <c r="H26" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="I26" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="J26" s="37" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J27" s="16"/>
+    </row>
+    <row r="28" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="3">
+      <c r="C28" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="17">
         <v>5</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="3">
-        <v>10</v>
-      </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="4">
-        <v>0</v>
-      </c>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J23" s="8"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="4">
-        <v>1</v>
-      </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="4">
-        <v>5</v>
-      </c>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J26" s="16"/>
-    </row>
-    <row r="27" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="17">
-        <v>5</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="J27" s="17" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="17">
-        <v>2</v>
-      </c>
       <c r="H28" s="18" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>11</v>
@@ -1914,27 +1961,27 @@
         <v>2</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>154</v>
+        <v>86</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>11</v>
@@ -1943,60 +1990,62 @@
         <v>8</v>
       </c>
       <c r="G30" s="17">
+        <v>2</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="17">
         <v>3</v>
       </c>
-      <c r="H30" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="17">
-        <v>0</v>
-      </c>
       <c r="H31" s="18" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="J31" s="17"/>
+        <v>89</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="32" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B32" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E32" s="17" t="s">
         <v>11</v>
@@ -2008,25 +2057,25 @@
         <v>0</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I32" s="18" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="J32" s="17"/>
     </row>
     <row r="33" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E33" s="17" t="s">
         <v>11</v>
@@ -2038,120 +2087,120 @@
         <v>0</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="J33" s="17"/>
     </row>
     <row r="34" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B34" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="17">
+        <v>0</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J34" s="17"/>
+    </row>
+    <row r="35" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="17">
+      <c r="B35" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="17">
         <v>1</v>
       </c>
-      <c r="H34" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="I34" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="J34" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J35" s="9"/>
-    </row>
-    <row r="36" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="H35" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J35" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J36" s="9"/>
+    </row>
+    <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="3">
+      <c r="C37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="3">
         <v>5</v>
       </c>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="4">
-        <v>2</v>
-      </c>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>40</v>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>11</v>
@@ -2160,81 +2209,79 @@
         <v>8</v>
       </c>
       <c r="G38" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J39" s="16"/>
-    </row>
-    <row r="40" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="4">
+        <v>1</v>
+      </c>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J40" s="16"/>
+    </row>
+    <row r="41" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B41" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" s="20">
+      <c r="C41" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="20">
         <v>2</v>
       </c>
-      <c r="H40" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="I40" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="J40" s="20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="20">
-        <v>1</v>
-      </c>
       <c r="H41" s="20" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="I41" s="20" t="s">
-        <v>36</v>
+        <v>117</v>
       </c>
       <c r="J41" s="20" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -2245,203 +2292,203 @@
         <v>9</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="E42" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G42" s="20">
+        <v>1</v>
+      </c>
+      <c r="H42" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I42" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J42" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="20">
         <v>2</v>
       </c>
-      <c r="H42" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="I42" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="J42" s="20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
+      <c r="H43" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="I43" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="J43" s="20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="33" t="s">
+      <c r="B44" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G43" s="17">
+      <c r="C44" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="17">
         <v>0</v>
       </c>
-      <c r="H43" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="I43" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J43" s="17"/>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J44" s="16"/>
-    </row>
-    <row r="45" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F45" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G45" s="20">
-        <v>2</v>
-      </c>
-      <c r="H45" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="I45" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="J45" s="20" t="s">
-        <v>160</v>
-      </c>
+      <c r="H44" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J44" s="17"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J45" s="16"/>
     </row>
     <row r="46" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="E46" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G46" s="20">
         <v>2</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="J46" s="20" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="C47" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="20">
+        <v>2</v>
+      </c>
+      <c r="H47" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="I47" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J47" s="20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="E47" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F47" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" s="20">
+      <c r="C48" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="20">
         <v>1</v>
       </c>
-      <c r="H47" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="I47" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J47" s="20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G48" s="17">
-        <v>8</v>
-      </c>
-      <c r="H48" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="I48" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="J48" s="17" t="s">
-        <v>162</v>
+      <c r="H48" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="I48" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="J48" s="20" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="E49" s="17" t="s">
         <v>11</v>
@@ -2453,92 +2500,92 @@
         <v>8</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="I49" s="18" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="J49" s="17" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="C50" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="17">
+        <v>8</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="I50" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="J50" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G50" s="17">
+      <c r="C51" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="17">
         <v>0</v>
       </c>
-      <c r="H50" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="I50" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="J50" s="17"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J51" s="16"/>
-    </row>
-    <row r="52" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" s="10">
-        <v>1</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="I52" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="J52" s="10" t="s">
-        <v>121</v>
-      </c>
+      <c r="H51" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I51" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J51" s="17"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J52" s="16"/>
     </row>
     <row r="53" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="E53" s="10" t="s">
         <v>8</v>
@@ -2547,48 +2594,80 @@
         <v>8</v>
       </c>
       <c r="G53" s="10">
+        <v>1</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="10">
         <v>2</v>
       </c>
-      <c r="H53" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="I53" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="J53" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B54" s="13" t="s">
+      <c r="H54" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G54" s="13">
+      <c r="C55" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="13">
         <v>0</v>
       </c>
-      <c r="H54" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="I54" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="J54" s="13" t="s">
-        <v>165</v>
+      <c r="H55" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J55" s="13" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving statistics changes fixed
</commit_message>
<xml_diff>
--- a/docs/endpoints.xlsx
+++ b/docs/endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521915F8-FA44-4F61-9BDF-CAE2F1B5E7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699ACD07-21B8-4F85-9A10-CA7460333B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="330" windowWidth="38700" windowHeight="15345" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
+    <workbookView xWindow="-105" yWindow="10440" windowWidth="26010" windowHeight="10545" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -582,7 +582,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -651,6 +651,15 @@
       <b/>
       <sz val="11"/>
       <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -763,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -778,7 +787,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -805,6 +813,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1121,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1555BF42-8AEC-4F54-8DDE-B70EA6966B6F}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="C34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,39 +1181,39 @@
       <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="20">
-        <v>11</v>
-      </c>
-      <c r="H2" s="21" t="s">
+      <c r="E2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="19">
+        <v>11</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1269,313 +1281,313 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="17">
+      <c r="E5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="16">
         <v>2</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="17">
+      <c r="E6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="16">
         <v>2</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="17">
+      <c r="E7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="16">
         <v>2</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="17">
+      <c r="E8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="16">
         <v>2</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="17">
+      <c r="E9" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="16">
         <v>0</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J9" s="17"/>
-    </row>
-    <row r="10" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="17">
+      <c r="E10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="16">
         <v>0</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="24"/>
-    </row>
-    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="J10" s="23"/>
+    </row>
+    <row r="11" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="17">
+      <c r="E11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="16">
         <v>0</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J11" s="26"/>
-    </row>
-    <row r="12" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="17">
+      <c r="E12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="16">
         <v>0</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="17"/>
-    </row>
-    <row r="13" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="17">
+      <c r="E13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="16">
         <v>0</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="I13" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J13" s="17"/>
-    </row>
-    <row r="14" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="27">
+      <c r="E14" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="26">
         <v>1</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1614,545 +1626,545 @@
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+    <row r="17" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="17">
+      <c r="E17" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="16">
         <v>3</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="I17" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="16" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+    <row r="18" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="17">
+      <c r="E18" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="16">
         <v>1</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+    <row r="20" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="E20" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="34">
+      <c r="E20" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="33">
         <v>2</v>
       </c>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="I20" s="35" t="s">
+      <c r="I20" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="J20" s="34" t="s">
+      <c r="J20" s="33" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+    <row r="21" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="E21" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="34">
-        <v>8</v>
-      </c>
-      <c r="H21" s="35" t="s">
+      <c r="E21" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="33">
+        <v>8</v>
+      </c>
+      <c r="H21" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="I21" s="35" t="s">
+      <c r="I21" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="J21" s="34" t="s">
+      <c r="J21" s="33" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+    <row r="22" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="E22" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="34">
+      <c r="E22" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="33">
         <v>1</v>
       </c>
-      <c r="H22" s="35" t="s">
+      <c r="H22" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="I22" s="35" t="s">
+      <c r="I22" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="J22" s="34" t="s">
+      <c r="J22" s="33" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+    <row r="23" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="E23" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="34">
+      <c r="E23" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="33">
         <v>12</v>
       </c>
-      <c r="H23" s="35" t="s">
+      <c r="H23" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="I23" s="35" t="s">
+      <c r="I23" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="J23" s="34" t="s">
+      <c r="J23" s="33" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
+    <row r="24" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="E24" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="37">
+      <c r="E24" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="36">
         <v>0</v>
       </c>
-      <c r="H24" s="37" t="s">
+      <c r="H24" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="I24" s="38" t="s">
+      <c r="I24" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="J24" s="39"/>
-    </row>
-    <row r="25" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
+      <c r="J24" s="38"/>
+    </row>
+    <row r="25" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="37">
+      <c r="E25" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="36">
         <v>2</v>
       </c>
-      <c r="H25" s="38" t="s">
+      <c r="H25" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="I25" s="38" t="s">
+      <c r="I25" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="J25" s="37" t="s">
+      <c r="J25" s="36" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
+    <row r="26" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="E26" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="37">
+      <c r="E26" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="36">
         <v>6</v>
       </c>
-      <c r="H26" s="38" t="s">
+      <c r="H26" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="I26" s="38" t="s">
+      <c r="I26" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="J26" s="37" t="s">
+      <c r="J26" s="36" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J27" s="16"/>
-    </row>
-    <row r="28" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="17">
+      <c r="E28" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="16">
         <v>5</v>
       </c>
-      <c r="H28" s="18" t="s">
+      <c r="H28" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="I28" s="18" t="s">
+      <c r="I28" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="J28" s="17" t="s">
+      <c r="J28" s="16" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+    <row r="29" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="17">
+      <c r="E29" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="16">
         <v>2</v>
       </c>
-      <c r="H29" s="18" t="s">
+      <c r="H29" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I29" s="18" t="s">
+      <c r="I29" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="J29" s="17" t="s">
+      <c r="J29" s="16" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+    <row r="30" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="17">
+      <c r="E30" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="16">
         <v>2</v>
       </c>
-      <c r="H30" s="18" t="s">
+      <c r="H30" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I30" s="18" t="s">
+      <c r="I30" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="J30" s="17" t="s">
+      <c r="J30" s="16" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
+    <row r="31" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="17">
+      <c r="E31" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="16">
         <v>3</v>
       </c>
-      <c r="H31" s="18" t="s">
+      <c r="H31" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="I31" s="18" t="s">
+      <c r="I31" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="J31" s="17" t="s">
+      <c r="J31" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+    <row r="32" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="17">
+      <c r="E32" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="16">
         <v>0</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I32" s="18" t="s">
+      <c r="I32" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="J32" s="17"/>
-    </row>
-    <row r="33" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="J32" s="16"/>
+    </row>
+    <row r="33" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="17">
+      <c r="E33" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="16">
         <v>0</v>
       </c>
-      <c r="H33" s="18" t="s">
+      <c r="H33" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I33" s="18" t="s">
+      <c r="I33" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="J33" s="17"/>
-    </row>
-    <row r="34" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="J33" s="16"/>
+    </row>
+    <row r="34" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E34" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="17">
+      <c r="E34" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="16">
         <v>0</v>
       </c>
-      <c r="H34" s="18" t="s">
+      <c r="H34" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="18" t="s">
+      <c r="I34" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="J34" s="17"/>
-    </row>
-    <row r="35" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+      <c r="J34" s="16"/>
+    </row>
+    <row r="35" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="17">
+      <c r="E35" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="16">
         <v>1</v>
       </c>
-      <c r="H35" s="18" t="s">
+      <c r="H35" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I35" s="18" t="s">
+      <c r="I35" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J35" s="17" t="s">
+      <c r="J35" s="16" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2250,329 +2262,329 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J40" s="16"/>
-    </row>
-    <row r="41" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="s">
+      <c r="J40" s="15"/>
+    </row>
+    <row r="41" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E41" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="20">
+      <c r="E41" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="19">
         <v>2</v>
       </c>
-      <c r="H41" s="20" t="s">
+      <c r="H41" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="20" t="s">
+      <c r="I41" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="J41" s="20" t="s">
+      <c r="J41" s="19" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
+    <row r="42" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E42" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="20">
+      <c r="E42" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="19">
         <v>1</v>
       </c>
-      <c r="H42" s="20" t="s">
+      <c r="H42" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I42" s="20" t="s">
+      <c r="I42" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="J42" s="20" t="s">
+      <c r="J42" s="19" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
+    <row r="43" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D43" s="20" t="s">
+      <c r="D43" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E43" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G43" s="20">
+      <c r="E43" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="19">
         <v>2</v>
       </c>
-      <c r="H43" s="20" t="s">
+      <c r="H43" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="I43" s="20" t="s">
+      <c r="I43" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="J43" s="20" t="s">
+      <c r="J43" s="19" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="33" t="s">
+    <row r="44" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="33" t="s">
+      <c r="B44" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E44" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G44" s="17">
+      <c r="E44" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="16">
         <v>0</v>
       </c>
-      <c r="H44" s="17" t="s">
+      <c r="H44" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="I44" s="17" t="s">
+      <c r="I44" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J44" s="17"/>
+      <c r="J44" s="16"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J45" s="16"/>
-    </row>
-    <row r="46" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
+      <c r="J45" s="15"/>
+    </row>
+    <row r="46" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D46" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="E46" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="20">
+      <c r="E46" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="19">
         <v>2</v>
       </c>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="I46" s="21" t="s">
+      <c r="I46" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="J46" s="20" t="s">
+      <c r="J46" s="19" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
+    <row r="47" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D47" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="E47" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F47" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" s="20">
+      <c r="E47" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="19">
         <v>2</v>
       </c>
-      <c r="H47" s="21" t="s">
+      <c r="H47" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="I47" s="21" t="s">
+      <c r="I47" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="J47" s="20" t="s">
+      <c r="J47" s="19" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
+    <row r="48" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="C48" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D48" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="E48" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G48" s="20">
+      <c r="E48" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="19">
         <v>1</v>
       </c>
-      <c r="H48" s="21" t="s">
+      <c r="H48" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="I48" s="21" t="s">
+      <c r="I48" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="J48" s="20" t="s">
+      <c r="J48" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
+    <row r="49" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="C49" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E49" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G49" s="17">
-        <v>8</v>
-      </c>
-      <c r="H49" s="18" t="s">
+      <c r="E49" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="16">
+        <v>8</v>
+      </c>
+      <c r="H49" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="I49" s="18" t="s">
+      <c r="I49" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="J49" s="17" t="s">
+      <c r="J49" s="16" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+    <row r="50" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="E50" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G50" s="17">
-        <v>8</v>
-      </c>
-      <c r="H50" s="18" t="s">
+      <c r="E50" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="16">
+        <v>8</v>
+      </c>
+      <c r="H50" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="I50" s="18" t="s">
+      <c r="I50" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="J50" s="17" t="s">
+      <c r="J50" s="16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
+    <row r="51" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="C51" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="D51" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="E51" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G51" s="17">
+      <c r="E51" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="16">
         <v>0</v>
       </c>
-      <c r="H51" s="18" t="s">
+      <c r="H51" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I51" s="18" t="s">
+      <c r="I51" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="J51" s="17"/>
+      <c r="J51" s="16"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J52" s="16"/>
+      <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
@@ -2581,28 +2593,28 @@
       <c r="B53" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="E53" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G53" s="10">
+      <c r="E53" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="40">
         <v>1</v>
       </c>
-      <c r="H53" s="11" t="s">
+      <c r="H53" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="I53" s="11" t="s">
+      <c r="I53" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="J53" s="10" t="s">
+      <c r="J53" s="40" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2613,60 +2625,60 @@
       <c r="B54" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G54" s="10">
+      <c r="E54" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="40">
         <v>2</v>
       </c>
-      <c r="H54" s="11" t="s">
+      <c r="H54" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="I54" s="11" t="s">
+      <c r="I54" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="J54" s="10" t="s">
+      <c r="J54" s="40" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B55" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="E55" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F55" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G55" s="13">
+      <c r="E55" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="42">
         <v>0</v>
       </c>
-      <c r="H55" s="14" t="s">
+      <c r="H55" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="I55" s="14" t="s">
+      <c r="I55" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="J55" s="13" t="s">
+      <c r="J55" s="42" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reset password --> change password
</commit_message>
<xml_diff>
--- a/docs/endpoints.xlsx
+++ b/docs/endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EABA96-5BBF-45EC-922C-1C4D50CCE62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09987DA8-4A81-4665-8E95-E2DA7805C4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t>Make admin</t>
   </si>
   <si>
-    <t>Reset password</t>
-  </si>
-  <si>
     <t>Make driver</t>
   </si>
   <si>
@@ -551,18 +548,12 @@
     <t>Forgot password</t>
   </si>
   <si>
-    <t>UserRestartPasswordRequest</t>
-  </si>
-  <si>
     <t>token</t>
   </si>
   <si>
     <t>Token nie jest poprawny.</t>
   </si>
   <si>
-    <t>/api/users/restart-password</t>
-  </si>
-  <si>
     <t>/api/users/make-admin/{id}</t>
   </si>
   <si>
@@ -591,6 +582,15 @@
   </si>
   <si>
     <t>/api/settlements/report-bug/{id}</t>
+  </si>
+  <si>
+    <t>/api/users/change-password</t>
+  </si>
+  <si>
+    <t>Change password</t>
+  </si>
+  <si>
+    <t>UserChangePasswordRequest</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1141,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1183,7 @@
         <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>20</v>
@@ -1206,7 +1206,7 @@
         <v>46</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F2" s="30"/>
       <c r="G2" s="7">
@@ -1219,7 +1219,7 @@
         <v>21</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -1230,26 +1230,26 @@
         <v>7</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="21">
         <v>3</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -1260,13 +1260,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="21">
@@ -1279,7 +1279,7 @@
         <v>26</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -1290,20 +1290,20 @@
         <v>16</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>52</v>
+        <v>183</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F5" s="32"/>
       <c r="G5" s="21">
         <v>0</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="I5" s="22" t="s">
         <v>26</v>
@@ -1382,7 +1382,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>51</v>
@@ -1414,10 +1414,10 @@
         <v>16</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>11</v>
@@ -1464,7 +1464,7 @@
         <v>26</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J10" s="4"/>
     </row>
@@ -1479,7 +1479,7 @@
         <v>41</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>11</v>
@@ -1494,7 +1494,7 @@
         <v>26</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J11" s="11"/>
     </row>
@@ -1509,7 +1509,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>11</v>
@@ -1524,7 +1524,7 @@
         <v>26</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J12" s="13"/>
     </row>
@@ -1539,7 +1539,7 @@
         <v>44</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>11</v>
@@ -1554,7 +1554,7 @@
         <v>26</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J13" s="4"/>
     </row>
@@ -1569,7 +1569,7 @@
         <v>45</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>11</v>
@@ -1584,7 +1584,7 @@
         <v>26</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14" s="4"/>
     </row>
@@ -1599,7 +1599,7 @@
         <v>43</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>11</v>
@@ -1625,19 +1625,19 @@
     </row>
     <row r="17" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="7">
@@ -1650,7 +1650,7 @@
         <v>26</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1664,10 +1664,10 @@
         <v>7</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>11</v>
@@ -1679,13 +1679,13 @@
         <v>3</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1696,10 +1696,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>11</v>
@@ -1711,7 +1711,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>22</v>
@@ -1731,10 +1731,10 @@
         <v>7</v>
       </c>
       <c r="C22" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>156</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>157</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>8</v>
@@ -1749,10 +1749,10 @@
         <v>36</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -1763,11 +1763,11 @@
         <v>7</v>
       </c>
       <c r="C23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D23" s="21" t="s">
-        <v>139</v>
-      </c>
       <c r="E23" s="21" t="s">
         <v>8</v>
       </c>
@@ -1778,13 +1778,13 @@
         <v>8</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J23" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -1795,10 +1795,10 @@
         <v>9</v>
       </c>
       <c r="C24" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="21" t="s">
         <v>135</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>136</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>8</v>
@@ -1816,7 +1816,7 @@
         <v>24</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -1827,10 +1827,10 @@
         <v>7</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E25" s="21" t="s">
         <v>8</v>
@@ -1842,13 +1842,13 @@
         <v>12</v>
       </c>
       <c r="H25" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="I25" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="I25" s="22" t="s">
-        <v>143</v>
-      </c>
       <c r="J25" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1859,10 +1859,10 @@
         <v>9</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E26" s="24" t="s">
         <v>11</v>
@@ -1874,10 +1874,10 @@
         <v>0</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J26" s="26"/>
     </row>
@@ -1889,10 +1889,10 @@
         <v>9</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E27" s="24" t="s">
         <v>11</v>
@@ -1907,10 +1907,10 @@
         <v>36</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1921,10 +1921,10 @@
         <v>16</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E28" s="24" t="s">
         <v>11</v>
@@ -1936,13 +1936,13 @@
         <v>6</v>
       </c>
       <c r="H28" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1956,10 +1956,10 @@
         <v>7</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>11</v>
@@ -1971,13 +1971,13 @@
         <v>5</v>
       </c>
       <c r="H30" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I30" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I30" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="J30" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1988,7 +1988,7 @@
         <v>16</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>48</v>
@@ -2006,10 +2006,10 @@
         <v>36</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2020,7 +2020,7 @@
         <v>16</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>49</v>
@@ -2038,10 +2038,10 @@
         <v>36</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2052,10 +2052,10 @@
         <v>16</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>11</v>
@@ -2067,13 +2067,13 @@
         <v>3</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2084,7 +2084,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>50</v>
@@ -2102,7 +2102,7 @@
         <v>26</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J34" s="4"/>
     </row>
@@ -2114,10 +2114,10 @@
         <v>9</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>11</v>
@@ -2132,7 +2132,7 @@
         <v>26</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J35" s="4"/>
     </row>
@@ -2144,10 +2144,10 @@
         <v>9</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>11</v>
@@ -2162,7 +2162,7 @@
         <v>26</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J36" s="4"/>
     </row>
@@ -2174,10 +2174,10 @@
         <v>17</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>11</v>
@@ -2195,7 +2195,7 @@
         <v>22</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2209,10 +2209,10 @@
         <v>7</v>
       </c>
       <c r="C39" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" s="21" t="s">
         <v>163</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>164</v>
       </c>
       <c r="E39" s="21" t="s">
         <v>8</v>
@@ -2224,13 +2224,13 @@
         <v>5</v>
       </c>
       <c r="H39" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I39" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J39" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>9</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D40" s="24" t="s">
         <v>50</v>
@@ -2256,10 +2256,10 @@
         <v>0</v>
       </c>
       <c r="H40" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I40" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J40" s="26"/>
     </row>
@@ -2271,10 +2271,10 @@
         <v>9</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E41" s="24" t="s">
         <v>11</v>
@@ -2289,10 +2289,10 @@
         <v>36</v>
       </c>
       <c r="I41" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J41" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2306,10 +2306,10 @@
         <v>7</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>8</v>
@@ -2321,13 +2321,13 @@
         <v>2</v>
       </c>
       <c r="H43" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I43" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="I43" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="J43" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2338,10 +2338,10 @@
         <v>9</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>8</v>
@@ -2359,7 +2359,7 @@
         <v>24</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2370,10 +2370,10 @@
         <v>9</v>
       </c>
       <c r="C45" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="E45" s="29" t="s">
         <v>8</v>
@@ -2383,13 +2383,13 @@
         <v>2</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2400,10 +2400,10 @@
         <v>9</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>11</v>
@@ -2415,7 +2415,7 @@
         <v>0</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>27</v>
@@ -2433,10 +2433,10 @@
         <v>9</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E48" s="29" t="s">
         <v>8</v>
@@ -2446,13 +2446,13 @@
         <v>2</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2463,10 +2463,10 @@
         <v>16</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>8</v>
@@ -2481,10 +2481,10 @@
         <v>36</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2495,10 +2495,10 @@
         <v>9</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>8</v>
@@ -2516,7 +2516,7 @@
         <v>24</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2527,10 +2527,10 @@
         <v>7</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>11</v>
@@ -2542,13 +2542,13 @@
         <v>8</v>
       </c>
       <c r="H51" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I51" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="I51" s="5" t="s">
-        <v>119</v>
-      </c>
       <c r="J51" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2559,10 +2559,10 @@
         <v>16</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>11</v>
@@ -2574,13 +2574,13 @@
         <v>8</v>
       </c>
       <c r="H52" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I52" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="I52" s="5" t="s">
-        <v>119</v>
-      </c>
       <c r="J52" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2591,10 +2591,10 @@
         <v>9</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>11</v>
@@ -2624,10 +2624,10 @@
         <v>9</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E55" s="31" t="s">
         <v>8</v>
@@ -2640,10 +2640,10 @@
         <v>36</v>
       </c>
       <c r="I55" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J55" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -2654,10 +2654,10 @@
         <v>9</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E56" s="31" t="s">
         <v>8</v>
@@ -2667,13 +2667,13 @@
         <v>2</v>
       </c>
       <c r="H56" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I56" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J56" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -2684,10 +2684,10 @@
         <v>9</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E57" s="24" t="s">
         <v>11</v>
@@ -2699,13 +2699,13 @@
         <v>0</v>
       </c>
       <c r="H57" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I57" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J57" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
super admin role added
</commit_message>
<xml_diff>
--- a/docs/endpoints.xlsx
+++ b/docs/endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB7E915-75A9-4F3C-96BA-E32F330DAA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44E5B7E-B602-40C6-B90E-669D880E9D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="192">
   <si>
     <t>Klasa</t>
   </si>
@@ -125,18 +125,9 @@
     <t>List&lt;SettlementsExtended&gt;</t>
   </si>
   <si>
-    <t>Brak użytkownika o id {id}.</t>
-  </si>
-  <si>
-    <t>Użytkownik zostało już wcześniej zablokowane. | Brak użytkownika o id {id}.</t>
-  </si>
-  <si>
     <t>Użytkownik jest już administratorem. | Brak użytkownika o id {id}.</t>
   </si>
   <si>
-    <t>Użytkownik nie jest zablokowany. | Brak użytkownika o id {id}.</t>
-  </si>
-  <si>
     <t>UserRequest</t>
   </si>
   <si>
@@ -146,9 +137,6 @@
     <t>Nic</t>
   </si>
   <si>
-    <t>Użytkownik jest już kierowcą. | Brak użytkownika o id {id}.</t>
-  </si>
-  <si>
     <t>/api/users/register</t>
   </si>
   <si>
@@ -1119,13 +1107,43 @@
       </rPr>
       <t xml:space="preserve"> | Link do zmiany hasła został już wysłany na ten adres email. Jest on nadal aktywny. | Brak możliwości zmiany hasła, konto nie zostało zweryfikowane. Link do weryfikacji został wysłany na podany adres email podczas rejestracji. | Brak możliwości wysłania linku do zmiany hasła. Spróbuj ponownie poźniej.</t>
     </r>
+  </si>
+  <si>
+    <t>super admin</t>
+  </si>
+  <si>
+    <t>/api/users/make-super-admin/{id}</t>
+  </si>
+  <si>
+    <t>Make super admin</t>
+  </si>
+  <si>
+    <t>Użytkownik jest już głównym administratorem. | Brak użytkownika od id {id}.</t>
+  </si>
+  <si>
+    <t>/api/users/find/super-admins</t>
+  </si>
+  <si>
+    <t>Find all super admins</t>
+  </si>
+  <si>
+    <t>Użytkownik jest już kierowcą. | Brak użytkownika o id {id}. | Nie możesz zdegradować głównego administratora do roli kierowcy.</t>
+  </si>
+  <si>
+    <t>Użytkownik nie jest zablokowany. | Brak użytkownika o id {id}. | Nie możesz zdegradować głównego administratora do roli administratora.</t>
+  </si>
+  <si>
+    <t>Użytkownik zostało już wcześniej zablokowane. | Brak użytkownika o id {id}. | Nie możesz zablokować głównego administratora.</t>
+  </si>
+  <si>
+    <t>Brak użytkownika o id {id}. | Nie możesz usunąć głównego administratora.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1208,6 +1226,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1229,7 +1257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1324,11 +1352,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1369,6 +1419,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1685,10 +1761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1555BF42-8AEC-4F54-8DDE-B70EA6966B6F}">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,15 +1775,16 @@
     <col min="4" max="4" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="255.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="255.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1727,19 +1804,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1747,29 +1827,30 @@
         <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="5">
-        <v>11</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>33</v>
+        <v>163</v>
+      </c>
+      <c r="F2" s="34"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="5">
+        <v>11</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
@@ -1777,29 +1858,30 @@
         <v>7</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="15">
+        <v>163</v>
+      </c>
+      <c r="F3" s="35"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="15">
         <v>4</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>61</v>
-      </c>
       <c r="I3" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
@@ -1807,29 +1889,30 @@
         <v>7</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="15">
+        <v>163</v>
+      </c>
+      <c r="F4" s="35"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="15">
         <v>5</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>26</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
@@ -1837,29 +1920,30 @@
         <v>16</v>
       </c>
       <c r="C5" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="F5" s="35"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="15">
+        <v>5</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="15">
-        <v>5</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1867,31 +1951,32 @@
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="3">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>35</v>
+      <c r="F6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="37"/>
+      <c r="H6" s="3">
+        <v>3</v>
       </c>
       <c r="I6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1899,31 +1984,32 @@
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="3">
-        <v>2</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>35</v>
+      <c r="F7" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="37"/>
+      <c r="H7" s="3">
+        <v>3</v>
       </c>
       <c r="I7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1931,31 +2017,32 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="3">
+        <v>46</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="3">
         <v>2</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="I8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1963,61 +2050,65 @@
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="3">
+        <v>184</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="37"/>
+      <c r="G9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="3">
         <v>2</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="I9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>26</v>
+      <c r="F10" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="37"/>
+      <c r="H10" s="3">
+        <v>3</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -2025,29 +2116,30 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="F11" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="37"/>
+      <c r="H11" s="3">
         <v>0</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -2055,29 +2147,30 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="F12" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="37"/>
+      <c r="H12" s="3">
         <v>0</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -2085,29 +2178,30 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="3">
+      <c r="F13" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="37"/>
+      <c r="H13" s="3">
         <v>0</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -2115,287 +2209,294 @@
         <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="37"/>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="37"/>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="37"/>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="43"/>
+      <c r="H17" s="9">
+        <v>2</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="F19" s="34"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" s="29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="37"/>
+      <c r="H21" s="3">
+        <v>3</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="4" t="s">
+      <c r="K21" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="9">
-        <v>1</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="10" t="s">
+      <c r="D22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="37"/>
+      <c r="H22" s="3">
+        <v>2</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
-    </row>
-    <row r="17" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="F17" s="31"/>
-      <c r="G17" s="5">
-        <v>1</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="27"/>
-    </row>
-    <row r="19" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="3">
-        <v>3</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="3">
-        <v>2</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="27"/>
-    </row>
-    <row r="22" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="15">
-        <v>2</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="15">
-        <v>8</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="J23" s="15" t="s">
+      <c r="K22" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="27"/>
+    </row>
+    <row r="24" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="15">
-        <v>1</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>35</v>
+      <c r="F24" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="33"/>
+      <c r="H24" s="15">
+        <v>2</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>10</v>
       </c>
@@ -2403,233 +2504,241 @@
         <v>7</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="15">
+      <c r="F25" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="33"/>
+      <c r="H25" s="15">
+        <v>8</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="33"/>
+      <c r="H26" s="15">
+        <v>1</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="33"/>
+      <c r="H27" s="15">
         <v>12</v>
       </c>
-      <c r="H25" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="J25" s="15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="18">
-        <v>0</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="I26" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="J26" s="20"/>
-    </row>
-    <row r="27" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="18">
-        <v>2</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="I27" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="41"/>
+      <c r="H28" s="18">
+        <v>0</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K28" s="20"/>
+    </row>
+    <row r="29" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="41"/>
+      <c r="H29" s="18">
+        <v>2</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J29" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="K29" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="18">
+      <c r="C30" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="41"/>
+      <c r="H30" s="18">
         <v>6</v>
       </c>
-      <c r="H28" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="I28" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="J28" s="18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="28"/>
-    </row>
-    <row r="30" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="3">
-        <v>5</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="3">
-        <v>2</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="K30" s="18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="28"/>
+    </row>
+    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="3">
-        <v>2</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>35</v>
+      <c r="F32" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="37"/>
+      <c r="H32" s="3">
+        <v>5</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>18</v>
       </c>
@@ -2637,91 +2746,98 @@
         <v>16</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>166</v>
+        <v>64</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="3">
-        <v>3</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>73</v>
+      <c r="F33" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="37"/>
+      <c r="H33" s="3">
+        <v>2</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="3">
-        <v>0</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>26</v>
+      <c r="F34" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="37"/>
+      <c r="H34" s="3">
+        <v>2</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>76</v>
+        <v>162</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="3">
-        <v>0</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>26</v>
+      <c r="F35" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="37"/>
+      <c r="H35" s="3">
+        <v>3</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J35" s="3"/>
-    </row>
-    <row r="36" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
@@ -2729,377 +2845,389 @@
         <v>9</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="3">
+      <c r="F36" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="37"/>
+      <c r="H36" s="3">
         <v>0</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="I36" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I36" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J36" s="3"/>
-    </row>
-    <row r="37" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="37"/>
+      <c r="H37" s="3">
+        <v>0</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="37"/>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="3">
+      <c r="C39" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="37"/>
+      <c r="H39" s="3">
         <v>2</v>
       </c>
-      <c r="H37" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I37" s="4" t="s">
+      <c r="I39" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J39" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J37" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="27"/>
-    </row>
-    <row r="39" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
+      <c r="K39" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="27"/>
+    </row>
+    <row r="41" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B41" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C41" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="33"/>
+      <c r="H41" s="15">
+        <v>5</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="J41" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="K41" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="41"/>
+      <c r="H42" s="18">
+        <v>0</v>
+      </c>
+      <c r="I42" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="J42" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="K42" s="20"/>
+    </row>
+    <row r="43" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D43" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="D39" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="15">
-        <v>5</v>
-      </c>
-      <c r="H39" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="I39" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="J39" s="15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="18" t="s">
+      <c r="E43" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="41"/>
+      <c r="H43" s="18">
+        <v>1</v>
+      </c>
+      <c r="I43" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J43" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="K43" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="28"/>
+    </row>
+    <row r="45" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="31"/>
+      <c r="H45" s="5">
+        <v>2</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" s="18">
+      <c r="C46" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="31"/>
+      <c r="H46" s="5">
+        <v>1</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="34"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="5">
+        <v>2</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="37"/>
+      <c r="H48" s="3">
         <v>0</v>
       </c>
-      <c r="H40" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="I40" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="J40" s="20"/>
-    </row>
-    <row r="41" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G41" s="18">
-        <v>1</v>
-      </c>
-      <c r="H41" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="I41" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="J41" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="28"/>
-    </row>
-    <row r="43" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" s="5">
-        <v>2</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="5">
-        <v>1</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E45" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="F45" s="31"/>
-      <c r="G45" s="5">
-        <v>2</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="3">
-        <v>0</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="I46" s="3" t="s">
+      <c r="I48" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J48" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J46" s="3"/>
-    </row>
-    <row r="47" spans="1:10" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="28"/>
-    </row>
-    <row r="48" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" s="31"/>
-      <c r="G48" s="5">
-        <v>2</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G49" s="5">
-        <v>2</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="1:11" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="28"/>
+    </row>
+    <row r="50" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>14</v>
       </c>
@@ -3107,239 +3235,352 @@
         <v>9</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D50" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="34"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="5">
+        <v>2</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="31"/>
+      <c r="H51" s="5">
+        <v>2</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E50" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G50" s="5">
+      <c r="D52" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="31"/>
+      <c r="H52" s="5">
         <v>1</v>
       </c>
-      <c r="H50" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I50" s="6" t="s">
+      <c r="I52" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J52" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J50" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G51" s="3">
-        <v>8</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" s="3">
-        <v>8</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K52" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="37"/>
+      <c r="H53" s="3">
+        <v>8</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="37"/>
+      <c r="H54" s="3">
+        <v>8</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G53" s="3">
+      <c r="C55" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="37"/>
+      <c r="H55" s="3">
         <v>0</v>
       </c>
-      <c r="H53" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I53" s="4" t="s">
+      <c r="I55" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J55" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J53" s="3"/>
-    </row>
-    <row r="54" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="26"/>
-      <c r="I54" s="26"/>
-      <c r="J54" s="28"/>
-    </row>
-    <row r="55" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
+      <c r="K55" s="3"/>
+    </row>
+    <row r="56" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="26"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="28"/>
+    </row>
+    <row r="57" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B57" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D55" s="15" t="s">
+      <c r="C57" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="35"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="15">
+        <v>1</v>
+      </c>
+      <c r="I57" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J57" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="K57" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E58" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="35"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="15">
+        <v>2</v>
+      </c>
+      <c r="I58" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="J58" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K58" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G59" s="41"/>
+      <c r="H59" s="18">
+        <v>1</v>
+      </c>
+      <c r="I59" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="J59" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E55" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="F55" s="33"/>
-      <c r="G55" s="15">
-        <v>1</v>
-      </c>
-      <c r="H55" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="I55" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="J55" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D56" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E56" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="F56" s="33"/>
-      <c r="G56" s="15">
-        <v>2</v>
-      </c>
-      <c r="H56" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="I56" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="J56" s="15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B57" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C57" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D57" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E57" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G57" s="18">
-        <v>1</v>
-      </c>
-      <c r="H57" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="I57" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="J57" s="18" t="s">
-        <v>126</v>
+      <c r="K59" s="18" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E17:F17"/>
+  <mergeCells count="50">
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="F6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
onr exception added to Availability
</commit_message>
<xml_diff>
--- a/docs/endpoints.xlsx
+++ b/docs/endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44E5B7E-B602-40C6-B90E-669D880E9D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587AD352-BFCB-4C3B-B3E2-4B7F7EA8E205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
   </bookViews>
@@ -383,9 +383,6 @@
     <t>/api/availability/submit</t>
   </si>
   <si>
-    <t>Brak użytkowniak o id {user_id}. | Dyspozycyjność na następny tydzień została już złożona przez {imie} {nazwisko}.</t>
-  </si>
-  <si>
     <t>Brak użytkowniak o id {user_id}. | Brak złożonej dyspozycyjności dla {imie} {nazwisko} na dzień {data}.</t>
   </si>
   <si>
@@ -1137,6 +1134,9 @@
   </si>
   <si>
     <t>Brak użytkownika o id {id}. | Nie możesz usunąć głównego administratora.</t>
+  </si>
+  <si>
+    <t>Brak użytkowniak o id {user_id}. | Dyspozycyjność na następny tydzień została już złożona przez {imie} {nazwisko}. | Pomiędzy dwiema zmianami musisz mieć minimum 12h przerwy.</t>
   </si>
 </sst>
 </file>
@@ -1409,22 +1409,27 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1433,12 +1438,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1764,7 +1764,7 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F12" sqref="F12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,7 +1804,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>23</v>
@@ -1832,11 +1832,11 @@
       <c r="D2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="31"/>
+      <c r="E2" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" s="41"/>
+      <c r="G2" s="38"/>
       <c r="H2" s="5">
         <v>11</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>21</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -1864,10 +1864,10 @@
         <v>42</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="33"/>
+        <v>162</v>
+      </c>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
       <c r="H3" s="15">
         <v>4</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>54</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -1889,16 +1889,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="33"/>
+        <v>162</v>
+      </c>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="15">
         <v>5</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>26</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -1920,27 +1920,27 @@
         <v>16</v>
       </c>
       <c r="C5" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>168</v>
-      </c>
       <c r="E5" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="33"/>
+        <v>162</v>
+      </c>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="15">
         <v>5</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>26</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1959,10 +1959,10 @@
       <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="37"/>
+      <c r="F6" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="40"/>
       <c r="H6" s="3">
         <v>3</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>21</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1992,10 +1992,10 @@
       <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="37"/>
+      <c r="F7" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="40"/>
       <c r="H7" s="3">
         <v>3</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>21</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -2017,15 +2017,15 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="37"/>
+      <c r="E8" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="40"/>
       <c r="G8" s="3" t="s">
         <v>8</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -2050,15 +2050,15 @@
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="37"/>
+      <c r="E9" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="40"/>
       <c r="G9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>21</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -2083,7 +2083,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>47</v>
@@ -2091,10 +2091,10 @@
       <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="37"/>
+      <c r="F10" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="40"/>
       <c r="H10" s="3">
         <v>3</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>21</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -2124,10 +2124,10 @@
       <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="37"/>
+      <c r="F11" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="40"/>
       <c r="H11" s="3">
         <v>0</v>
       </c>
@@ -2155,10 +2155,10 @@
       <c r="E12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="37"/>
+      <c r="F12" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="40"/>
       <c r="H12" s="3">
         <v>0</v>
       </c>
@@ -2186,10 +2186,10 @@
       <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="37"/>
+      <c r="F13" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="40"/>
       <c r="H13" s="3">
         <v>0</v>
       </c>
@@ -2217,10 +2217,10 @@
       <c r="E14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="37"/>
+      <c r="F14" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="40"/>
       <c r="H14" s="3">
         <v>0</v>
       </c>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -2240,18 +2240,18 @@
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="E15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="37"/>
+      <c r="F15" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="40"/>
       <c r="H15" s="3">
         <v>0</v>
       </c>
@@ -2261,7 +2261,7 @@
       <c r="J15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K15" s="38"/>
+      <c r="K15" s="30"/>
     </row>
     <row r="16" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -2279,10 +2279,10 @@
       <c r="E16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="37"/>
+      <c r="F16" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="40"/>
       <c r="H16" s="3">
         <v>0</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>22</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2342,22 +2342,22 @@
     </row>
     <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="F19" s="34"/>
-      <c r="G19" s="31"/>
+        <v>153</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="F19" s="41"/>
+      <c r="G19" s="38"/>
       <c r="H19" s="5">
         <v>1</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>26</v>
       </c>
       <c r="K19" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2400,10 +2400,10 @@
       <c r="E21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="37"/>
+      <c r="F21" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="40"/>
       <c r="H21" s="3">
         <v>3</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>55</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2433,10 +2433,10 @@
       <c r="E22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="37"/>
+      <c r="F22" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="40"/>
       <c r="H22" s="3">
         <v>2</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>22</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -2471,18 +2471,18 @@
         <v>7</v>
       </c>
       <c r="C24" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>145</v>
-      </c>
       <c r="E24" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="33"/>
+      <c r="G24" s="34"/>
       <c r="H24" s="15">
         <v>2</v>
       </c>
@@ -2490,10 +2490,10 @@
         <v>32</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2504,29 +2504,29 @@
         <v>7</v>
       </c>
       <c r="C25" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="15" t="s">
-        <v>127</v>
-      </c>
       <c r="E25" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="33"/>
+      <c r="G25" s="34"/>
       <c r="H25" s="15">
         <v>8</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -2537,18 +2537,18 @@
         <v>9</v>
       </c>
       <c r="C26" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="15" t="s">
-        <v>124</v>
-      </c>
       <c r="E26" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F26" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="33"/>
+      <c r="G26" s="34"/>
       <c r="H26" s="15">
         <v>1</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>24</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2570,10 +2570,10 @@
         <v>7</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>8</v>
@@ -2581,18 +2581,18 @@
       <c r="F27" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="33"/>
+      <c r="G27" s="34"/>
       <c r="H27" s="15">
         <v>12</v>
       </c>
       <c r="I27" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="J27" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="J27" s="16" t="s">
-        <v>131</v>
-      </c>
       <c r="K27" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2603,18 +2603,18 @@
         <v>9</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="41"/>
+      <c r="F28" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="36"/>
       <c r="H28" s="18">
         <v>0</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>86</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K28" s="20"/>
     </row>
@@ -2634,7 +2634,7 @@
         <v>9</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>102</v>
@@ -2642,10 +2642,10 @@
       <c r="E29" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="41"/>
+      <c r="F29" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="36"/>
       <c r="H29" s="18">
         <v>2</v>
       </c>
@@ -2653,10 +2653,10 @@
         <v>32</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2667,29 +2667,29 @@
         <v>16</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="41"/>
+      <c r="F30" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="36"/>
       <c r="H30" s="18">
         <v>6</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K30" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -2721,10 +2721,10 @@
       <c r="E32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="37"/>
+      <c r="F32" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="40"/>
       <c r="H32" s="3">
         <v>5</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>68</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2754,10 +2754,10 @@
       <c r="E33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="37"/>
+      <c r="F33" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="40"/>
       <c r="H33" s="3">
         <v>2</v>
       </c>
@@ -2787,10 +2787,10 @@
       <c r="E34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="37"/>
+      <c r="F34" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="40"/>
       <c r="H34" s="3">
         <v>2</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>16</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>66</v>
@@ -2820,10 +2820,10 @@
       <c r="E35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="37"/>
+      <c r="F35" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="40"/>
       <c r="H35" s="3">
         <v>3</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>68</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2853,10 +2853,10 @@
       <c r="E36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="37"/>
+      <c r="F36" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="40"/>
       <c r="H36" s="3">
         <v>0</v>
       </c>
@@ -2884,10 +2884,10 @@
       <c r="E37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="37"/>
+      <c r="F37" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="40"/>
       <c r="H37" s="3">
         <v>0</v>
       </c>
@@ -2915,10 +2915,10 @@
       <c r="E38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="37"/>
+      <c r="F38" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="40"/>
       <c r="H38" s="3">
         <v>0</v>
       </c>
@@ -2946,10 +2946,10 @@
       <c r="E39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" s="37"/>
+      <c r="F39" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="40"/>
       <c r="H39" s="3">
         <v>2</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>22</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -2984,29 +2984,29 @@
         <v>7</v>
       </c>
       <c r="C41" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="15" t="s">
-        <v>150</v>
-      </c>
       <c r="E41" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F41" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G41" s="33"/>
+      <c r="G41" s="34"/>
       <c r="H41" s="15">
         <v>5</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K41" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -3017,7 +3017,7 @@
         <v>9</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>45</v>
@@ -3025,10 +3025,10 @@
       <c r="E42" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="41"/>
+      <c r="F42" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="36"/>
       <c r="H42" s="18">
         <v>0</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>86</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K42" s="20"/>
     </row>
@@ -3048,18 +3048,18 @@
         <v>9</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E43" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F43" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="G43" s="41"/>
+      <c r="F43" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="36"/>
       <c r="H43" s="18">
         <v>1</v>
       </c>
@@ -3067,10 +3067,10 @@
         <v>32</v>
       </c>
       <c r="J43" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K43" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -3102,12 +3102,12 @@
       <c r="E45" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F45" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="31"/>
+      <c r="F45" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="38"/>
       <c r="H45" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>94</v>
@@ -3116,7 +3116,7 @@
         <v>95</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>115</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3135,10 +3135,10 @@
       <c r="E46" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F46" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" s="31"/>
+      <c r="F46" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="38"/>
       <c r="H46" s="5">
         <v>1</v>
       </c>
@@ -3165,11 +3165,11 @@
       <c r="D47" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E47" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="F47" s="34"/>
-      <c r="G47" s="31"/>
+      <c r="E47" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="41"/>
+      <c r="G47" s="38"/>
       <c r="H47" s="5">
         <v>2</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>85</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3199,10 +3199,10 @@
       <c r="E48" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G48" s="37"/>
+      <c r="F48" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="40"/>
       <c r="H48" s="3">
         <v>0</v>
       </c>
@@ -3240,11 +3240,11 @@
       <c r="D50" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E50" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" s="34"/>
-      <c r="G50" s="31"/>
+      <c r="E50" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="41"/>
+      <c r="G50" s="38"/>
       <c r="H50" s="5">
         <v>2</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>110</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3266,7 +3266,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>103</v>
@@ -3274,10 +3274,10 @@
       <c r="E51" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F51" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G51" s="31"/>
+      <c r="F51" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="38"/>
       <c r="H51" s="5">
         <v>2</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>110</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3307,10 +3307,10 @@
       <c r="E52" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F52" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G52" s="31"/>
+      <c r="F52" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="38"/>
       <c r="H52" s="5">
         <v>1</v>
       </c>
@@ -3340,10 +3340,10 @@
       <c r="E53" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G53" s="37"/>
+      <c r="F53" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="40"/>
       <c r="H53" s="3">
         <v>8</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>110</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3373,10 +3373,10 @@
       <c r="E54" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G54" s="37"/>
+      <c r="F54" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="40"/>
       <c r="H54" s="3">
         <v>8</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>110</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3406,10 +3406,10 @@
       <c r="E55" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F55" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G55" s="37"/>
+      <c r="F55" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="40"/>
       <c r="H55" s="3">
         <v>0</v>
       </c>
@@ -3450,8 +3450,8 @@
       <c r="E57" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F57" s="35"/>
-      <c r="G57" s="33"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="34"/>
       <c r="H57" s="15">
         <v>1</v>
       </c>
@@ -3481,8 +3481,8 @@
       <c r="E58" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F58" s="35"/>
-      <c r="G58" s="33"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="34"/>
       <c r="H58" s="15">
         <v>2</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>83</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -3512,10 +3512,10 @@
       <c r="E59" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="G59" s="41"/>
+      <c r="F59" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G59" s="36"/>
       <c r="H59" s="18">
         <v>1</v>
       </c>
@@ -3526,44 +3526,16 @@
         <v>82</v>
       </c>
       <c r="K59" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="E19:G19"/>
@@ -3576,11 +3548,39 @@
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
one more exception handled
</commit_message>
<xml_diff>
--- a/docs/endpoints.xlsx
+++ b/docs/endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B38BC7-C5A4-4E54-99CC-DC310841A19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3FBEFC-8E1E-4789-851F-120EDC10FB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8835" yWindow="1875" windowWidth="28800" windowHeight="13575" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
   </bookViews>
@@ -1059,9 +1059,6 @@
     <t>Brak użytkownika o id {id}. | Nie możesz usunąć głównego administratora.</t>
   </si>
   <si>
-    <t>Brak użytkowniak o id {user_id}. | Dyspozycyjność na następny tydzień została już złożona przez {imie} {nazwisko}. | Pomiędzy dwiema zmianami musisz mieć minimum 12h przerwy.</t>
-  </si>
-  <si>
     <t>/api/shifts/find/car-unavailable</t>
   </si>
   <si>
@@ -1164,6 +1161,9 @@
   </si>
   <si>
     <t>/api/accidents/change-guilt/{id}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brak użytkowniak o id {user_id}. | Dyspozycyjność na następny tydzień została już złożona przez {imie} {nazwisko}. | Pomiędzy dwiema zmianami musisz mieć minimum 12h przerwy. | Dyspozycyjność na następny tydzień mogła zostać zgłoszona do końca czwartku. </t>
   </si>
 </sst>
 </file>
@@ -1444,10 +1444,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1457,18 +1463,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1484,6 +1478,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1802,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1555BF42-8AEC-4F54-8DDE-B70EA6966B6F}">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="K30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,8 +1874,8 @@
       <c r="E2" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="5">
         <v>11</v>
       </c>
@@ -1902,11 +1902,11 @@
       <c r="D3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
       <c r="H3" s="15">
         <v>4</v>
       </c>
@@ -1933,11 +1933,11 @@
       <c r="D4" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="15">
         <v>5</v>
       </c>
@@ -1964,11 +1964,11 @@
       <c r="D5" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="40"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="15">
         <v>5</v>
       </c>
@@ -1998,10 +1998,10 @@
       <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="42"/>
+      <c r="F6" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="39"/>
       <c r="H6" s="3">
         <v>3</v>
       </c>
@@ -2031,10 +2031,10 @@
       <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="42"/>
+      <c r="F7" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="39"/>
       <c r="H7" s="3">
         <v>3</v>
       </c>
@@ -2061,10 +2061,10 @@
       <c r="D8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="42"/>
+      <c r="E8" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="39"/>
       <c r="G8" s="3" t="s">
         <v>8</v>
       </c>
@@ -2094,10 +2094,10 @@
       <c r="D9" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="E9" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="42"/>
+      <c r="E9" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="39"/>
       <c r="G9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2130,10 +2130,10 @@
       <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="42"/>
+      <c r="F10" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="39"/>
       <c r="H10" s="3">
         <v>3</v>
       </c>
@@ -2163,10 +2163,10 @@
       <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="42"/>
+      <c r="F11" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="39"/>
       <c r="H11" s="3">
         <v>0</v>
       </c>
@@ -2194,10 +2194,10 @@
       <c r="E12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="42"/>
+      <c r="F12" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="39"/>
       <c r="H12" s="3">
         <v>0</v>
       </c>
@@ -2225,10 +2225,10 @@
       <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="42"/>
+      <c r="F13" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="39"/>
       <c r="H13" s="3">
         <v>0</v>
       </c>
@@ -2256,10 +2256,10 @@
       <c r="E14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="42"/>
+      <c r="F14" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="39"/>
       <c r="H14" s="3">
         <v>0</v>
       </c>
@@ -2287,10 +2287,10 @@
       <c r="E15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="42"/>
+      <c r="F15" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="39"/>
       <c r="H15" s="3">
         <v>0</v>
       </c>
@@ -2318,10 +2318,10 @@
       <c r="E16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="42"/>
+      <c r="F16" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="39"/>
       <c r="H16" s="3">
         <v>0</v>
       </c>
@@ -2349,10 +2349,10 @@
       <c r="E17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="44"/>
+      <c r="F17" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="49"/>
       <c r="H17" s="9">
         <v>2</v>
       </c>
@@ -2395,8 +2395,8 @@
       <c r="E19" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="36"/>
       <c r="H19" s="5">
         <v>1</v>
       </c>
@@ -2439,10 +2439,10 @@
       <c r="E21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="42"/>
+      <c r="F21" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="39"/>
       <c r="H21" s="3">
         <v>3</v>
       </c>
@@ -2472,10 +2472,10 @@
       <c r="E22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="42"/>
+      <c r="F22" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="39"/>
       <c r="H22" s="3">
         <v>2</v>
       </c>
@@ -2518,10 +2518,10 @@
       <c r="E24" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="40"/>
+      <c r="F24" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="42"/>
       <c r="H24" s="15">
         <v>2</v>
       </c>
@@ -2551,10 +2551,10 @@
       <c r="E25" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="40"/>
+      <c r="F25" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="42"/>
       <c r="H25" s="15">
         <v>9</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>130</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -2584,10 +2584,10 @@
       <c r="E26" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="40"/>
+      <c r="F26" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="42"/>
       <c r="H26" s="15">
         <v>1</v>
       </c>
@@ -2617,10 +2617,10 @@
       <c r="E27" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="40"/>
+      <c r="F27" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="42"/>
       <c r="H27" s="15">
         <v>12</v>
       </c>
@@ -2650,10 +2650,10 @@
       <c r="E28" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="46"/>
+      <c r="F28" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="44"/>
       <c r="H28" s="18">
         <v>0</v>
       </c>
@@ -2681,10 +2681,10 @@
       <c r="E29" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="46"/>
+      <c r="F29" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="44"/>
       <c r="H29" s="18">
         <v>2</v>
       </c>
@@ -2714,10 +2714,10 @@
       <c r="E30" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="48"/>
+      <c r="F30" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="46"/>
       <c r="H30" s="32">
         <v>6</v>
       </c>
@@ -2739,23 +2739,23 @@
         <v>9</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="49"/>
+      <c r="F31" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="47"/>
       <c r="H31" s="18">
         <v>0</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J31" s="18" t="s">
         <v>133</v>
@@ -2791,10 +2791,10 @@
       <c r="E33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="42"/>
+      <c r="F33" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="39"/>
       <c r="H33" s="3">
         <v>5</v>
       </c>
@@ -2824,10 +2824,10 @@
       <c r="E34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="42"/>
+      <c r="F34" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="39"/>
       <c r="H34" s="3">
         <v>2</v>
       </c>
@@ -2857,10 +2857,10 @@
       <c r="E35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="42"/>
+      <c r="F35" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="39"/>
       <c r="H35" s="3">
         <v>2</v>
       </c>
@@ -2890,10 +2890,10 @@
       <c r="E36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="42"/>
+      <c r="F36" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="39"/>
       <c r="H36" s="3">
         <v>3</v>
       </c>
@@ -2923,10 +2923,10 @@
       <c r="E37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="42"/>
+      <c r="F37" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="39"/>
       <c r="H37" s="3">
         <v>0</v>
       </c>
@@ -2954,10 +2954,10 @@
       <c r="E38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="42"/>
+      <c r="F38" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="39"/>
       <c r="H38" s="3">
         <v>0</v>
       </c>
@@ -2985,10 +2985,10 @@
       <c r="E39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" s="42"/>
+      <c r="F39" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="39"/>
       <c r="H39" s="3">
         <v>0</v>
       </c>
@@ -3016,10 +3016,10 @@
       <c r="E40" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" s="42"/>
+      <c r="F40" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="39"/>
       <c r="H40" s="3">
         <v>2</v>
       </c>
@@ -3062,10 +3062,10 @@
       <c r="E42" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F42" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="40"/>
+      <c r="F42" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="42"/>
       <c r="H42" s="15">
         <v>8</v>
       </c>
@@ -3087,18 +3087,18 @@
         <v>16</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E43" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F43" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="G43" s="46"/>
+      <c r="F43" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="44"/>
       <c r="H43" s="18">
         <v>1</v>
       </c>
@@ -3120,29 +3120,29 @@
         <v>9</v>
       </c>
       <c r="C44" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D44" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="D44" s="18" t="s">
-        <v>196</v>
-      </c>
       <c r="E44" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="G44" s="46"/>
+      <c r="F44" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="44"/>
       <c r="H44" s="18">
         <v>8</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J44" s="19" t="s">
         <v>140</v>
       </c>
       <c r="K44" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -3161,10 +3161,10 @@
       <c r="E45" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F45" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="G45" s="46"/>
+      <c r="F45" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="44"/>
       <c r="H45" s="18">
         <v>0</v>
       </c>
@@ -3192,10 +3192,10 @@
       <c r="E46" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F46" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="46"/>
+      <c r="F46" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="44"/>
       <c r="H46" s="18">
         <v>1</v>
       </c>
@@ -3241,9 +3241,9 @@
       <c r="F48" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G48" s="37"/>
+      <c r="G48" s="36"/>
       <c r="H48" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>94</v>
@@ -3252,7 +3252,7 @@
         <v>95</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
       <c r="F49" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="37"/>
+      <c r="G49" s="36"/>
       <c r="H49" s="5">
         <v>1</v>
       </c>
@@ -3304,8 +3304,8 @@
       <c r="E50" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F50" s="36"/>
-      <c r="G50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="36"/>
       <c r="H50" s="5">
         <v>2</v>
       </c>
@@ -3335,10 +3335,10 @@
       <c r="E51" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F51" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G51" s="42"/>
+      <c r="F51" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="39"/>
       <c r="H51" s="3">
         <v>0</v>
       </c>
@@ -3379,8 +3379,8 @@
       <c r="E53" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F53" s="36"/>
-      <c r="G53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="36"/>
       <c r="H53" s="5">
         <v>2</v>
       </c>
@@ -3413,7 +3413,7 @@
       <c r="F54" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G54" s="37"/>
+      <c r="G54" s="36"/>
       <c r="H54" s="5">
         <v>2</v>
       </c>
@@ -3446,7 +3446,7 @@
       <c r="F55" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G55" s="37"/>
+      <c r="G55" s="36"/>
       <c r="H55" s="5">
         <v>1</v>
       </c>
@@ -3476,10 +3476,10 @@
       <c r="E56" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G56" s="42"/>
+      <c r="F56" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="39"/>
       <c r="H56" s="3">
         <v>8</v>
       </c>
@@ -3509,10 +3509,10 @@
       <c r="E57" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F57" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G57" s="42"/>
+      <c r="F57" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57" s="39"/>
       <c r="H57" s="3">
         <v>8</v>
       </c>
@@ -3542,10 +3542,10 @@
       <c r="E58" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F58" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G58" s="42"/>
+      <c r="F58" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="39"/>
       <c r="H58" s="3">
         <v>0</v>
       </c>
@@ -3583,11 +3583,11 @@
       <c r="D60" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E60" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="F60" s="39"/>
-      <c r="G60" s="40"/>
+      <c r="E60" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="41"/>
+      <c r="G60" s="42"/>
       <c r="H60" s="15">
         <v>1</v>
       </c>
@@ -3614,11 +3614,11 @@
       <c r="D61" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E61" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="F61" s="39"/>
-      <c r="G61" s="40"/>
+      <c r="E61" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="41"/>
+      <c r="G61" s="42"/>
       <c r="H61" s="15">
         <v>2</v>
       </c>
@@ -3648,10 +3648,10 @@
       <c r="E62" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="G62" s="46"/>
+      <c r="F62" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="44"/>
       <c r="H62" s="18">
         <v>1</v>
       </c>
@@ -3667,42 +3667,11 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="E19:G19"/>
@@ -3715,11 +3684,42 @@
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="E53:G53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
configuration and logout done
</commit_message>
<xml_diff>
--- a/docs/endpoints.xlsx
+++ b/docs/endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3FBEFC-8E1E-4789-851F-120EDC10FB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113AA0FA-F54D-48E5-8973-0CCE88AB81BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8835" yWindow="1875" windowWidth="28800" windowHeight="13575" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="203">
   <si>
     <t>Klasa</t>
   </si>
@@ -1164,6 +1164,12 @@
   </si>
   <si>
     <t xml:space="preserve">Brak użytkowniak o id {user_id}. | Dyspozycyjność na następny tydzień została już złożona przez {imie} {nazwisko}. | Pomiędzy dwiema zmianami musisz mieć minimum 12h przerwy. | Dyspozycyjność na następny tydzień mogła zostać zgłoszona do końca czwartku. </t>
+  </si>
+  <si>
+    <t>/api/users/logout</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
 </sst>
 </file>
@@ -1800,10 +1806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1555BF42-8AEC-4F54-8DDE-B70EA6966B6F}">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,10 +1934,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>163</v>
+        <v>201</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>154</v>
+        <v>202</v>
       </c>
       <c r="E4" s="40" t="s">
         <v>162</v>
@@ -1939,30 +1945,28 @@
       <c r="F4" s="41"/>
       <c r="G4" s="42"/>
       <c r="H4" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>179</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="E5" s="40" t="s">
         <v>162</v>
@@ -1973,46 +1977,44 @@
         <v>5</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>168</v>
+        <v>26</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>26</v>
       </c>
       <c r="K5" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="F6" s="41"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="15">
+        <v>5</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="15" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="3">
-        <v>3</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2023,10 +2025,10 @@
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
@@ -2045,10 +2047,10 @@
         <v>21</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -2056,20 +2058,20 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>157</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="39"/>
       <c r="H8" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>32</v>
@@ -2078,10 +2080,10 @@
         <v>21</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -2089,10 +2091,10 @@
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>182</v>
+        <v>46</v>
       </c>
       <c r="E9" s="38" t="s">
         <v>11</v>
@@ -2111,10 +2113,10 @@
         <v>21</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -2122,20 +2124,20 @@
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="39"/>
+        <v>182</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="39"/>
+      <c r="G10" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="H10" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>32</v>
@@ -2144,7 +2146,7 @@
         <v>21</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -2152,13 +2154,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>11</v>
@@ -2168,15 +2170,17 @@
       </c>
       <c r="G11" s="39"/>
       <c r="H11" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K11" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="12" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -2186,10 +2190,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>11</v>
@@ -2217,10 +2221,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>11</v>
@@ -2248,10 +2252,10 @@
         <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>11</v>
@@ -2271,7 +2275,7 @@
       </c>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -2279,10 +2283,10 @@
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>184</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>185</v>
+        <v>50</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>11</v>
@@ -2300,9 +2304,9 @@
       <c r="J15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K15" s="30"/>
-    </row>
-    <row r="16" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
@@ -2310,10 +2314,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>11</v>
@@ -2331,143 +2335,141 @@
       <c r="J16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="3"/>
+      <c r="K16" s="30"/>
     </row>
     <row r="17" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="39"/>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C18" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="48" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="49"/>
-      <c r="H17" s="9">
+      <c r="E18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="49"/>
+      <c r="H18" s="9">
         <v>2</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J18" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="K18" s="9" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="27"/>
-    </row>
-    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:11" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E20" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="F19" s="37"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="5">
+      <c r="F20" s="37"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="5">
         <v>1</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K19" s="29" t="s">
+      <c r="K20" s="29" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="27"/>
-    </row>
-    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="39"/>
-      <c r="H21" s="3">
-        <v>3</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>177</v>
-      </c>
+    <row r="21" spans="1:11" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="27"/>
     </row>
     <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>11</v>
@@ -2477,63 +2479,63 @@
       </c>
       <c r="G22" s="39"/>
       <c r="H22" s="3">
+        <v>3</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="39"/>
+      <c r="H23" s="3">
         <v>2</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="27"/>
-    </row>
-    <row r="24" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="42"/>
-      <c r="H24" s="15">
-        <v>2</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" s="15" t="s">
-        <v>145</v>
-      </c>
+    <row r="24" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="27"/>
     </row>
     <row r="25" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
@@ -2543,10 +2545,10 @@
         <v>7</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>8</v>
@@ -2556,30 +2558,30 @@
       </c>
       <c r="G25" s="42"/>
       <c r="H25" s="15">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>8</v>
@@ -2589,30 +2591,30 @@
       </c>
       <c r="G26" s="42"/>
       <c r="H26" s="15">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>24</v>
+        <v>130</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>8</v>
@@ -2622,48 +2624,50 @@
       </c>
       <c r="G27" s="42"/>
       <c r="H27" s="15">
+        <v>1</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="42"/>
+      <c r="H28" s="15">
         <v>12</v>
       </c>
-      <c r="I27" s="16" t="s">
+      <c r="I28" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="J27" s="16" t="s">
+      <c r="J28" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="K28" s="15" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="44"/>
-      <c r="H28" s="18">
-        <v>0</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="J28" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="K28" s="20"/>
     </row>
     <row r="29" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
@@ -2673,10 +2677,10 @@
         <v>9</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>11</v>
@@ -2686,140 +2690,138 @@
       </c>
       <c r="G29" s="44"/>
       <c r="H29" s="18">
+        <v>0</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="J29" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="K29" s="20"/>
+    </row>
+    <row r="30" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="44"/>
+      <c r="H30" s="18">
         <v>2</v>
       </c>
-      <c r="I29" s="19" t="s">
+      <c r="I30" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J30" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="K29" s="18" t="s">
+      <c r="K30" s="18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+    <row r="31" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B31" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C31" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="D31" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="E30" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="46"/>
-      <c r="H30" s="32">
+      <c r="E31" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="46"/>
+      <c r="H31" s="32">
         <v>6</v>
       </c>
-      <c r="I30" s="33" t="s">
+      <c r="I31" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="J30" s="33" t="s">
+      <c r="J31" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="K30" s="32" t="s">
+      <c r="K31" s="32" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+    <row r="32" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B32" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C32" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D32" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="E31" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="47"/>
-      <c r="H31" s="18">
+      <c r="E32" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="47"/>
+      <c r="H32" s="18">
         <v>0</v>
       </c>
-      <c r="I31" s="18" t="s">
+      <c r="I32" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="J32" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="K31" s="18"/>
-    </row>
-    <row r="32" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="27"/>
-    </row>
-    <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="39"/>
-      <c r="H33" s="3">
-        <v>5</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="18"/>
+    </row>
+    <row r="33" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="27"/>
+    </row>
+    <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>11</v>
@@ -2829,16 +2831,16 @@
       </c>
       <c r="G34" s="39"/>
       <c r="H34" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>68</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>61</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2849,10 +2851,10 @@
         <v>16</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>11</v>
@@ -2871,10 +2873,10 @@
         <v>68</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
@@ -2882,10 +2884,10 @@
         <v>16</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>161</v>
+        <v>65</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>11</v>
@@ -2895,30 +2897,30 @@
       </c>
       <c r="G36" s="39"/>
       <c r="H36" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>68</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>71</v>
+        <v>161</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>11</v>
@@ -2928,15 +2930,17 @@
       </c>
       <c r="G37" s="39"/>
       <c r="H37" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K37" s="3"/>
+        <v>68</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="38" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
@@ -2946,10 +2950,10 @@
         <v>9</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>11</v>
@@ -2977,10 +2981,10 @@
         <v>9</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>11</v>
@@ -3005,13 +3009,13 @@
         <v>18</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>11</v>
@@ -3021,95 +3025,93 @@
       </c>
       <c r="G40" s="39"/>
       <c r="H40" s="3">
+        <v>0</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="39"/>
+      <c r="H41" s="3">
         <v>2</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I41" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="J41" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K40" s="3" t="s">
+      <c r="K41" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="27"/>
-    </row>
-    <row r="42" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+    <row r="42" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="27"/>
+    </row>
+    <row r="43" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B43" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C43" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D43" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="E42" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F42" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="42"/>
-      <c r="H42" s="15">
-        <v>8</v>
-      </c>
-      <c r="I42" s="16" t="s">
+      <c r="E43" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="42"/>
+      <c r="H43" s="15">
+        <v>8</v>
+      </c>
+      <c r="I43" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="J42" s="16" t="s">
+      <c r="J43" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="K42" s="15" t="s">
+      <c r="K43" s="15" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="G43" s="44"/>
-      <c r="H43" s="18">
-        <v>1</v>
-      </c>
-      <c r="I43" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J43" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="K43" s="18" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -3117,13 +3119,13 @@
         <v>13</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E44" s="18" t="s">
         <v>11</v>
@@ -3133,16 +3135,16 @@
       </c>
       <c r="G44" s="44"/>
       <c r="H44" s="18">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>197</v>
+        <v>32</v>
       </c>
       <c r="J44" s="19" t="s">
         <v>140</v>
       </c>
       <c r="K44" s="18" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -3153,10 +3155,10 @@
         <v>9</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>150</v>
+        <v>194</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>45</v>
+        <v>195</v>
       </c>
       <c r="E45" s="18" t="s">
         <v>11</v>
@@ -3166,15 +3168,17 @@
       </c>
       <c r="G45" s="44"/>
       <c r="H45" s="18">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I45" s="19" t="s">
-        <v>86</v>
+        <v>197</v>
       </c>
       <c r="J45" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="K45" s="20"/>
+        <v>140</v>
+      </c>
+      <c r="K45" s="18" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="46" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
@@ -3184,10 +3188,10 @@
         <v>9</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>152</v>
+        <v>45</v>
       </c>
       <c r="E46" s="18" t="s">
         <v>11</v>
@@ -3197,76 +3201,74 @@
       </c>
       <c r="G46" s="44"/>
       <c r="H46" s="18">
+        <v>0</v>
+      </c>
+      <c r="I46" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="J46" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="K46" s="20"/>
+    </row>
+    <row r="47" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="44"/>
+      <c r="H47" s="18">
         <v>1</v>
       </c>
-      <c r="I46" s="19" t="s">
+      <c r="I47" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="J46" s="19" t="s">
+      <c r="J47" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="K46" s="18" t="s">
+      <c r="K47" s="18" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="28"/>
-    </row>
-    <row r="48" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
+    <row r="48" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="28"/>
+    </row>
+    <row r="49" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B49" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C49" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="G48" s="36"/>
-      <c r="H48" s="5">
-        <v>4</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="K48" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>8</v>
@@ -3276,16 +3278,16 @@
       </c>
       <c r="G49" s="36"/>
       <c r="H49" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>84</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3296,135 +3298,135 @@
         <v>9</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E50" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" s="37"/>
+        <v>89</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="G50" s="36"/>
       <c r="H50" s="5">
+        <v>1</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="37"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="5">
         <v>2</v>
       </c>
-      <c r="I50" s="5" t="s">
+      <c r="I51" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J50" s="5" t="s">
+      <c r="J51" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="K50" s="5" t="s">
+      <c r="K51" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
+    <row r="52" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B52" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="G51" s="39"/>
-      <c r="H51" s="3">
+      <c r="E52" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="39"/>
+      <c r="H52" s="3">
         <v>0</v>
       </c>
-      <c r="I51" s="3" t="s">
+      <c r="I52" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="J51" s="3" t="s">
+      <c r="J52" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K51" s="3"/>
-    </row>
-    <row r="52" spans="1:11" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="26"/>
-      <c r="J52" s="26"/>
-      <c r="K52" s="28"/>
-    </row>
-    <row r="53" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E53" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" s="37"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="5">
-        <v>2</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="J53" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="K53" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:11" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="28"/>
     </row>
     <row r="54" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>165</v>
+        <v>111</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F54" s="35" t="s">
-        <v>11</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E54" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="37"/>
       <c r="G54" s="36"/>
       <c r="H54" s="5">
         <v>2</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="J54" s="6" t="s">
         <v>110</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3432,13 +3434,13 @@
         <v>14</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>108</v>
+        <v>165</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>8</v>
@@ -3448,49 +3450,49 @@
       </c>
       <c r="G55" s="36"/>
       <c r="H55" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I55" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J55" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" s="36"/>
+      <c r="H56" s="5">
+        <v>1</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J56" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K55" s="5" t="s">
+      <c r="K56" s="5" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F56" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="G56" s="39"/>
-      <c r="H56" s="3">
-        <v>8</v>
-      </c>
-      <c r="I56" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="K56" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3498,13 +3500,13 @@
         <v>14</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>11</v>
@@ -3523,7 +3525,7 @@
         <v>110</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3531,13 +3533,13 @@
         <v>14</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>11</v>
@@ -3547,59 +3549,61 @@
       </c>
       <c r="G58" s="39"/>
       <c r="H58" s="3">
+        <v>8</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G59" s="39"/>
+      <c r="H59" s="3">
         <v>0</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="I59" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J58" s="4" t="s">
+      <c r="J59" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K58" s="3"/>
-    </row>
-    <row r="59" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="26"/>
-      <c r="I59" s="26"/>
-      <c r="J59" s="26"/>
-      <c r="K59" s="28"/>
-    </row>
-    <row r="60" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D60" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E60" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="F60" s="41"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="15">
-        <v>1</v>
-      </c>
-      <c r="I60" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J60" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="K60" s="15" t="s">
-        <v>84</v>
-      </c>
+      <c r="K59" s="3"/>
+    </row>
+    <row r="60" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="26"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="26"/>
+      <c r="J60" s="26"/>
+      <c r="K60" s="28"/>
     </row>
     <row r="61" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
@@ -3609,10 +3613,10 @@
         <v>9</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E61" s="40" t="s">
         <v>8</v>
@@ -3620,106 +3624,138 @@
       <c r="F61" s="41"/>
       <c r="G61" s="42"/>
       <c r="H61" s="15">
+        <v>1</v>
+      </c>
+      <c r="I61" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J61" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="K61" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E62" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="41"/>
+      <c r="G62" s="42"/>
+      <c r="H62" s="15">
         <v>2</v>
       </c>
-      <c r="I61" s="16" t="s">
+      <c r="I62" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J61" s="16" t="s">
+      <c r="J62" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K61" s="15" t="s">
+      <c r="K62" s="15" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
+    <row r="63" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="B63" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C62" s="18" t="s">
+      <c r="C63" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D62" s="18" t="s">
+      <c r="D63" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E62" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F62" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="G62" s="44"/>
-      <c r="H62" s="18">
+      <c r="E63" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="44"/>
+      <c r="H63" s="18">
         <v>1</v>
       </c>
-      <c r="I62" s="19" t="s">
+      <c r="I63" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J62" s="19" t="s">
+      <c r="J63" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="K62" s="18" t="s">
+      <c r="K63" s="18" t="s">
         <v>121</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="54">
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E6:G6"/>
     <mergeCell ref="E5:G5"/>
+    <mergeCell ref="F7:G7"/>
     <mergeCell ref="E4:G4"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="F11:G11"/>
+    <mergeCell ref="E20:G20"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F23:G23"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F33:G33"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F32:G32"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
     <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
     <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="E60:G60"/>
     <mergeCell ref="E61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="F63:G63"/>
     <mergeCell ref="F55:G55"/>
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="F57:G57"/>
     <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F59:G59"/>
     <mergeCell ref="F49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="E54:G54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>